<commit_message>
added section three of report
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="221">
   <si>
     <t xml:space="preserve">Profession</t>
   </si>
@@ -60,7 +60,7 @@
     <t xml:space="preserve">Civil</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE LAW = yes, LIKE PHYSICS = yes</t>
+    <t xml:space="preserve">LIKE SOCIAL SCIENCE = yes, LIKE PHYSICS = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Petroleum</t>
@@ -165,7 +165,7 @@
     <t xml:space="preserve">Oncology</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE CHESMISTRY =yes</t>
+    <t xml:space="preserve">LIKE CHEMISTRY =yes</t>
   </si>
   <si>
     <t xml:space="preserve">Orthopedics</t>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">Cardiology</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE STATE LICENSURE = yes, LIKE chemistry = yes</t>
+    <t xml:space="preserve">STATE LICENSURE = yes, LIKE chemistry = yes</t>
   </si>
   <si>
     <t xml:space="preserve">General Practitioner</t>
@@ -201,7 +201,7 @@
     <t xml:space="preserve">Journalism</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE MEDIA = yes, LIKE SOCIOLOGY = yes</t>
+    <t xml:space="preserve">LIKE MEDIA = yes, LIKE SOCIAL SCIENCE = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Editing</t>
@@ -303,13 +303,13 @@
     <t xml:space="preserve">Farm Ownership</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE FARMING = yes, LIKE MANAGEMENT = yes</t>
+    <t xml:space="preserve">GOOD CREDIT, LIKE MANAGEMENT = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Ranch Work</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE BUSINESS = yes, LIKE MANAGEMENT = yes</t>
+    <t xml:space="preserve">GROUP WORK = yes, LIKE MANAGEMENT = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Viniculture</t>
@@ -327,7 +327,7 @@
     <t xml:space="preserve">Irigation</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE SOIL = yes</t>
+    <t xml:space="preserve">LIKE WATER RESOURCES = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Health Care</t>
@@ -381,7 +381,7 @@
     <t xml:space="preserve">K-12</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE WRITING = yes, LIKE READING = yes, LIKE COMMUNICATIONS = yes</t>
+    <t xml:space="preserve">LIKE READING = yes, LIKE COMMUNICATIONS = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Higher Education</t>
@@ -441,13 +441,13 @@
     <t xml:space="preserve">AI</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE MATH = yes, LIKE OPTIMIZATION = yes</t>
+    <t xml:space="preserve">LIKE MATH = yes,SOCIAL SCIENCE = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Machine Learning</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE MATH = yes, LIKE DATA ANALYSIS = yes</t>
+    <t xml:space="preserve">LIKE MATH = yes, LIKE ANALYTICAL SKILLS = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Software Engineering</t>
@@ -456,7 +456,7 @@
     <t xml:space="preserve">Data Science</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE MATH = yes, LIKE PROBLEM SOLVING = yes</t>
+    <t xml:space="preserve">LIKE MATH = yes, LIKE MARKETING = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Languages</t>
@@ -585,61 +585,55 @@
     <t xml:space="preserve">IF DEGREE = computer science AND GOOD GRADES = true AND GROUP WORK = true THEN PROFESSION = computer science</t>
   </si>
   <si>
+    <t xml:space="preserve">Clause Variable List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE PHYSICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = engineering AND LIKE MATH = yes LIKE MATH = yes, LIKE PHYSICS = yes LIKE PHYSICS = yes THEN AREA = electrical engineering</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIKE MATH</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE PHYSICS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE LAW</t>
+    <t xml:space="preserve">IF DEGREE = engineering AND LIKE PHYSICS = yes AND GROUP WORK = yes then AREA = mechanical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = engineering AND LIKE LAW = yes AND LIKE PHYSICS = yes the AREA = CIVIL</t>
   </si>
   <si>
     <t xml:space="preserve">LIKE BIOLOGY</t>
   </si>
   <si>
+    <t xml:space="preserve">IF DEGREE = engineering AND LIKE MATH = yes AND LIKE BIOLOGY = yes THEN AREA = petroleum engineering</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIKE CHEMISTRY</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE ASTROPHYSICS</t>
+    <t xml:space="preserve">IF DEGREE = engineering AND LIKE CHEMISTRY = yes AND GROUP WORK = yes THEN AREA = chemical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MARKETING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = science AND LIKE BIOLOGY = yes AND LIKE CHEMISTRY= yes THEN AREA = pharmaceuticals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MANAGEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = science</t>
   </si>
   <si>
     <t xml:space="preserve">GOOD CREDIT</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE ACCOUNTING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE TAXATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MARKETING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MANAGEMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTERED NURSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE RESIDENCY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE GOOD CREDIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE PHARMACOLOGY</t>
-  </si>
-  <si>
     <t xml:space="preserve">LIKE MEDICAL ETHICS</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE STATE LICENSURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE HEMODYNAMIC STUDIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE ARTS</t>
+    <t xml:space="preserve">STATE LICENSURE</t>
   </si>
   <si>
     <t xml:space="preserve">LIKE WRITING</t>
@@ -648,16 +642,49 @@
     <t xml:space="preserve">LIKE ORIGINALITY</t>
   </si>
   <si>
+    <t xml:space="preserve">LIKE MEDIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE SOCIAL SCIENCE</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIKE ENGLISH</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE MEDIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE SOCIOLOGY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE COMMUNICATIONS</t>
+    <t xml:space="preserve">LIKE READING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE CLIMATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE STONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE LAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE SOIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE WATER RESOURCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE ANALYTICAL SKILLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE INTERNSHIPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE ANATOMY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELIABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE REPAIRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AREA</t>
   </si>
 </sst>
 </file>
@@ -909,8 +936,8 @@
   </sheetPr>
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2364,17 +2391,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="131.020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1224489795918"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -2386,7 +2413,7 @@
         <v>148</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2412,139 +2439,184 @@
       <c r="Y1" s="9"/>
       <c r="Z1" s="9"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>188</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>190</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>193</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>195</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>199</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>201</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>202</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>196</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed rule base for fc knowledge base
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="273">
   <si>
     <t xml:space="preserve">Profession</t>
   </si>
@@ -87,7 +87,7 @@
     <t xml:space="preserve">Biology</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE PHYSICS = yes, LIKE CHEMISTRY= yes</t>
+    <t xml:space="preserve">LIKE BIOLOGY = yes, LIKE GROUP WORK = yes</t>
   </si>
   <si>
     <t xml:space="preserve">LABWORK = yes</t>
@@ -120,7 +120,7 @@
     <t xml:space="preserve">Business Owner</t>
   </si>
   <si>
-    <t xml:space="preserve">GOOD CREDIT = yes, </t>
+    <t xml:space="preserve">GOOD CREDIT = yes</t>
   </si>
   <si>
     <t xml:space="preserve">LEADERSHIP = yes</t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
-    <t xml:space="preserve">GROUP WORK = yes,</t>
+    <t xml:space="preserve">GROUP WORK = yes</t>
   </si>
   <si>
     <t xml:space="preserve">CEO</t>
@@ -153,10 +153,7 @@
     <t xml:space="preserve">Medical</t>
   </si>
   <si>
-    <t xml:space="preserve">Mental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP WORK = yes</t>
+    <t xml:space="preserve">Mental Health</t>
   </si>
   <si>
     <t xml:space="preserve">MED SCHOOL = yes</t>
@@ -207,7 +204,7 @@
     <t xml:space="preserve">Editing</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE ENGLISH = yes, LIKE WRITING = yes, </t>
+    <t xml:space="preserve">LIKE ENGLISH = yes, LIKE READING = yes, </t>
   </si>
   <si>
     <t xml:space="preserve">Copy Writing</t>
@@ -285,7 +282,7 @@
     <t xml:space="preserve">Accessability</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE GROUP WORK = yes, LIKE SOCIAL SCIENCE</t>
+    <t xml:space="preserve">LIKE GROUP WORK = yes, LIKE SOCIAL SCIENCE = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Clinical Psychology</t>
@@ -303,9 +300,6 @@
     <t xml:space="preserve">Farm Ownership</t>
   </si>
   <si>
-    <t xml:space="preserve">GOOD CREDIT, LIKE MANAGEMENT = yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ranch Work</t>
   </si>
   <si>
@@ -372,319 +366,481 @@
     <t xml:space="preserve">Early Childhood</t>
   </si>
   <si>
+    <t xml:space="preserve">LIKE CHILDREN = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TECHER CERTIFICATE = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE READING = yes, LIKE COMMUNICATIONS = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Higher Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MATH = yes,  LIKE CHEMISTRY = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teacher's Aid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE COMMUNICATIONS = yes, LIKE CHILDREN = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counselor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE SOCIAL SCIENCE = yes, LIKE COMMUNICATION = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propety Managemement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MANAGEMENT = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTDOOR WORK = no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELIABLE = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintenance Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE REPAIRS = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Painting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEGREE = computer science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MATH = yes,SOCIAL SCIENCE = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MATH = yes, LIKE ANALYTICAL SKILLS = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MATH = yes, LIKE MARKETING = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE ORIGINALITY = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause Variable Lise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEGREE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF GPA &gt;= 3.5 THEN GOOD GRADES = true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOOD GRADES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF GPA &lt; 3.5 THEN GOOD GRADES = false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LABWORK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF COURSES WITH LABS &gt; 2 THEN LABWORK = true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEADERSHIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF GROUP LEADER &gt;= 1 THEN LEADERSHIP = true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED SCHOOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = engineering AND GOOD GRADES = true THEN PROFESSION = engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP WORK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = science AND GOOD GRADES = true AND LABWORK = true THEN PROFESSION = science </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORK ALONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE != none AND LEADERSHIP = true THEN PROFESSION = business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTDOOR WORK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF GROUP WORK = false THEN WORK ALONE = true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDICAL CERTIFICATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE != none AND MED SCHOOL = true AND GROUP WORK = true THEN PROFESSION = medical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COURSES WITH LABS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEACHER CERTIFICATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = english AND WORK ALONE = true THEN PROFESSION = english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF HOURS OUTSIDE &gt;= 16 THEN OUTDOOR WORK = true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROFESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = science AND OUTDOOR WOORK = true THEN PROFESSION = geography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = psychology AND GROUP WORK = true THEN PROFESSION = psychology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP LEADER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = none AND OUTDOOR WORK = true THEN PROFESSION = agriculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOURS OUTSIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF MED SCHOOL = false and MED FIELD = true THEN MEDICAL CERTIFICATE = true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED FIELD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE != none AND MEDICAL CERTIFICATE = true AND GROUP WORK = true THEN PROFESSION = health care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRIMINAL BACKGROUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF CRIMINAL BACKGROUND = true THEN TEACHER CERTIFICATE = false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE != none AND TEACHER CERTIFICATE = true THEN PROFESSION = education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = none AND OUTDOOR WORK = false THEN PROFESSION = property management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF DEGREE = computer science AND GOOD GRADES = true AND GROUP WORK = true THEN PROFESSION = computer science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause Variable List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE PHYSICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = engineering AND LIKE MATH = yes LIKE MATH = yes, LIKE PHYSICS = yes LIKE PHYSICS = yes THEN AREA = electrical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MATH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = engineering AND LIKE PHYSICS = yes AND GROUP WORK = yes then AREA = mechanical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = engineering AND LIKE LAW = yes AND LIKE PHYSICS = yes the AREA = CIVIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE BIOLOGY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = engineering AND LIKE MATH = yes AND LIKE BIOLOGY = yes THEN AREA = petroleum engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE CHEMISTRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = engineering AND LIKE CHEMISTRY = yes AND GROUP WORK = yes THEN AREA = chemical engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MARKETING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = science AND LIKE BIOLOGY = yes AND LIKE CHEMISTRY= yes THEN AREA = pharmaceuticals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MANAGEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = science AND LIKE BIOLOGY = yes AND LIKE GROUP WORK = yes THEN AREA = biology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOOD CREDIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = science AND LIKE MATH =yes THEN AREA = astronomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MEDICAL ETHICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = science AND LIKE PHYSICS = yes THEN AREA = quantam physics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATE LICENSURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = science AND LIKE BIOLOGY = yes AND LIKE PHYSICS = yes THEN area = oceanography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE WRITING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = business AND GOOD CREDIT = yes THEN AREA = business owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE ORIGINALITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = business AND LIKE MARKETING = yes AND LIKE MANAGEMENT = yes THEN AREA = manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE MEDIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = business AND LIKE MATH = yes THEN AREA = accounting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE SOCIAL SCIENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = business AND GROUP WORK = yes THEN AREA = human resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE ENGLISH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = business AND GOOD CREDIT = yes, LIKE MANAGEMENT = yes THEN AREA = ceo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = medical AND GROUP WORK = yes THEN AREA = mental health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE READING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = medical LIKE CHEMISTRY =yes THEN AREA = oncology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE CLIMATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = medical AND STATE LICENSURE = yes AND LIKE chemistry = yes THEN AREA = cardiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE STONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = medical AND LIKE MEDICAL ETHICS = yes THEN AREA = orthopedics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE LAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = medical AND LIKE BIOLOGY = yes AND LIKE CHEMISTRY= yes THEN AREA = general practitioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE SOIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = english AND LIKE WRITING = yes AND LIKE ORIGINALITY = yes THEN AREA = author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE WATER RESOURCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = english AND LIKE MEDIA = yes AND LIKE SOCIAL SCIENCE = yes THEN AREA = journalism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE ANALYTICAL SKILLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = english AND LIKE ENGLISH = yes AND LIKE READING = yes THEN AREA = editing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE INTERNSHIPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = english AND LIKE MARKETING = yes AND LIKE ENGLISH = yes THEN AREA = copy writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE ANATOMY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = english AND LIKE READING = yes THEN LIKE ORIGINALITY = yes THEN AREA = academia</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIKE CHILDREN</t>
   </si>
   <si>
-    <t xml:space="preserve">TECHER CERTIFICATE = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE READING = yes, LIKE COMMUNICATIONS = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Higher Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MATH = yes,  LIKE CHEMISTRY = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teacher's Aid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE COMMUNICATIONS = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Counselor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE SOCIAL SCIENCE = yes, LIKE COMMUNICATION = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Propety Managemement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MANAGEMENT = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUTDOOR WORK = no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cleaning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELIABLE = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maintenance Work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE REPAIRS = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Painting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEGREE = computer science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MATH = yes,SOCIAL SCIENCE = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Machine Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MATH = yes, LIKE ANALYTICAL SKILLS = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MATH = yes, LIKE MARKETING = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Languages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE ORIGINALITY = yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clause Variable Lise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEGREE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF GPA &gt;= 3.5 THEN GOOD GRADES = true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOOD GRADES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF GPA &lt; 3.5 THEN GOOD GRADES = false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LABWORK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF COURSES WITH LABS &gt; 2 THEN LABWORK = true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEADERSHIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF GROUP LEADER &gt;= 1 THEN LEADERSHIP = true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MED SCHOOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = engineering AND GOOD GRADES = true THEN PROFESSION = engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP WORK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = science AND GOOD GRADES = true AND LABWORK = true THEN PROFESSION = science </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WORK ALONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE != none AND LEADERSHIP = true THEN PROFESSION = business</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUTDOOR WORK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF GROUP WORK = false THEN WORK ALONE = true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEDICAL CERTIFICATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE != none AND MED SCHOOL = true AND GROUP WORK = true THEN PROFESSION = medical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COURSES WITH LABS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEACHER CERTIFICATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = english AND WORK ALONE = true THEN PROFESSION = english</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF HOURS OUTSIDE &gt;= 16 THEN OUTDOOR WORK = true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROFESSION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = science AND OUTDOOR WOORK = true THEN PROFESSION = geography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = psychology AND GROUP WORK = true THEN PROFESSION = psychology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP LEADER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = none AND OUTDOOR WORK = true THEN PROFESSION = agriculture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOURS OUTSIDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF MED SCHOOL = false and MED FIELD = true THEN MEDICAL CERTIFICATE = true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MED FIELD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE != none AND MEDICAL CERTIFICATE = true AND GROUP WORK = true THEN PROFESSION = health care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRIMINAL BACKGROUND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF CRIMINAL BACKGROUND = true THEN TEACHER CERTIFICATE = false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE != none AND TEACHER CERTIFICATE = true THEN PROFESSION = education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = none AND OUTDOOR WORK = false THEN PROFESSION = property management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = computer science AND GOOD GRADES = true AND GROUP WORK = true THEN PROFESSION = computer science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clause Variable List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE PHYSICS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = engineering AND LIKE MATH = yes LIKE MATH = yes, LIKE PHYSICS = yes LIKE PHYSICS = yes THEN AREA = electrical engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MATH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = engineering AND LIKE PHYSICS = yes AND GROUP WORK = yes then AREA = mechanical engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = engineering AND LIKE LAW = yes AND LIKE PHYSICS = yes the AREA = CIVIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE BIOLOGY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = engineering AND LIKE MATH = yes AND LIKE BIOLOGY = yes THEN AREA = petroleum engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE CHEMISTRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = engineering AND LIKE CHEMISTRY = yes AND GROUP WORK = yes THEN AREA = chemical engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MARKETING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = science AND LIKE BIOLOGY = yes AND LIKE CHEMISTRY= yes THEN AREA = pharmaceuticals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MANAGEMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF DEGREE = science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOOD CREDIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MEDICAL ETHICS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STATE LICENSURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE WRITING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE ORIGINALITY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE MEDIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE SOCIAL SCIENCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE ENGLISH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE READING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE CLIMATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE STONES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE LAND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE SOIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE WATER RESOURCES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE ANALYTICAL SKILLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE INTERNSHIPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE ANATOMY</t>
+    <t xml:space="preserve">IF PROFESSION = geography AND LIKE CLIMATE = yes AND LIKE STONES = yes THEN AREA = precious metals</t>
   </si>
   <si>
     <t xml:space="preserve">RELIABLE</t>
   </si>
   <si>
+    <t xml:space="preserve">IF PROFESSION = geography AND LIKE LAND = yes AND LIKE ORIGINALITY = yes THEN AREA = cartography</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIKE REPAIRS</t>
   </si>
   <si>
+    <t xml:space="preserve">IF PROFESSION = geography AND LIKE SOIL = yes AND LIKE CLIMATE = yes THEN AREA = climatology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = geography AND LIKE WATER RESOURCES = yes AND LIKE SOIL = yes THEN AREA = environmental management</t>
+  </si>
+  <si>
     <t xml:space="preserve">AREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = geography AND LIKE MATH = yes THEN AREA = geomatics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = psychology AND LIKE SOCIAL SCIENCE = yes THEN AREA = mental therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = psychology AND LIKE GROUP WORK = yes AND LIKE ANALYTICAL SKILLS = yes THEN AREA = psychological research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = psychology AND LIKE INTERNSHIPS = yes THEN AREA = industrial psychology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = psychology AND LIKE GROUP WORK = yes AND LIKE SOCIAL SCIENCE = yes THEN AREA = accessibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = psychology AND LIKE COMMUNICATION = yes, LIKE ANALYTICAL SKILLS = yes THEN AREA = clinical psychology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = agriculture AND GOOD CREDIT = yes AND LIKE MANAGEMENT = yes THEN AREA = farm ownership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = agriculture AND GROUP WORK = yes AND LIKE MANAGEMENT = yes THEN AREA = ranch work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = agriculture AND LIKE MANAGEMENT = yes AND LIKE MARKETING = yes THEN AREA = viniculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = agriculture AND LIKE CHEMISTRY = yes THEN AREA = crop spraying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = agriculture AND LIKE WATER RESOURCES = yes THEN AREA = irrigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = health care AND LIKE COMMUNICATION = yes THEN AREA = health services management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = health care AND LIKE ADMINISTRATION = yes THEN AREA = health care administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = health care AND LIKE BIOLOGY = yes THEN AREA = physicians assistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = health care AND LIKE ADMINISTRATION = yes AND LIKE GROUP WORK = yes THEN AREA = public health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = health care AND LIKE ANATOMY = yes AND LIKE CHEMISTRY = yes THEN AREA = nursing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = education AND LIKE CHILDREN = yes THEN AREA = early childhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = education AND LIKE READING = yes AND LIKE COMMUNICATIONS = yes THEN AREA = k-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = education AND LIKE MATH = yes AND  LIKE CHEMISTRY = yes THEN AREA = higher education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = education AND LIKE COMMUNICATIONS = yes, LIKE CHILDREN = yes THEN AREA = teacher’s aid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = education AND LIKE SOCIAL SCIENCE = yes AND LIKE COMMUNICATION = yes THEN AREA = counselor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = property management AND LIKE MANAGEMENT = yes THEN AREA = property manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = property management AND GROUP WORK = yes THEN AREA = realty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = property management AND RELIABLE = yes THEN AREA = cleaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = property management AND LIKE REPAIRS = yes THEN AREA = maintenance work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = property management AND LIKE COMMUNICATION = yes THEN AREA = painting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = cs AND LIKE MATH = yes AND SOCIAL SCIENCE = yes THEN AREA = ai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = cs AND LIKE MATH = yes AND LIKE ANALYTICAL SKILLS = yes THEN AREA = machine learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = cs AND GROUP WORK = yes THEN AREA = software engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = cs AND LIKE MATH = yes AND LIKE MARKETING = yes THEN AREA = data science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF PROFESSION = cs AND LIKE ORIGINALITY = yes THEN AREA = languages</t>
   </si>
 </sst>
 </file>
@@ -936,14 +1092,15 @@
   </sheetPr>
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.7295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.2551020408163"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="109.071428571429"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.9030612244898"/>
   </cols>
@@ -1171,7 +1328,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="3" t="s">
@@ -1181,7 +1338,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3" t="s">
@@ -1235,48 +1392,48 @@
         <v>43</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>19</v>
@@ -1307,58 +1464,58 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -1386,57 +1543,57 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>37</v>
@@ -1467,58 +1624,58 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -1546,58 +1703,58 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -1625,60 +1782,60 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
       <c r="B43" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
       <c r="B44" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -1706,58 +1863,58 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
       <c r="B48" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -1785,58 +1942,58 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="B53" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -1864,16 +2021,16 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,42 +2039,42 @@
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
       <c r="B59" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -1975,13 +2132,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>149</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2009,191 +2166,191 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,32 +2358,32 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,12 +2391,12 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2247,7 +2404,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2255,12 +2412,12 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,12 +2425,12 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,12 +2438,12 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2294,12 +2451,12 @@
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2307,17 +2464,17 @@
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,7 +2482,7 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,12 +2490,12 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,12 +2503,12 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,17 +2516,17 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2391,10 +2548,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B61" activeCellId="0" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2407,13 +2564,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2441,63 +2598,63 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>200</v>
@@ -2505,10 +2662,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,107 +2673,317 @@
         <v>203</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>208</v>
+        <v>213</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>209</v>
+        <v>216</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>210</v>
+        <v>218</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>211</v>
+        <v>220</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>212</v>
+        <v>222</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>213</v>
+        <v>224</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>214</v>
+        <v>226</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>215</v>
+        <v>228</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>216</v>
+        <v>230</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>217</v>
+        <v>232</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>116</v>
+        <v>234</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>218</v>
+        <v>236</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>219</v>
+        <v>238</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>150</v>
+        <v>171</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>220</v>
+        <v>241</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="0" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added forward chaining clause variable list
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="275">
   <si>
     <t xml:space="preserve">Profession</t>
   </si>
@@ -339,7 +339,7 @@
     <t xml:space="preserve">Healthcare Administration</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE ADMINISTRATION = yes</t>
+    <t xml:space="preserve">LIKE MANAGEMENT = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Physician Assistant</t>
@@ -351,7 +351,7 @@
     <t xml:space="preserve">Public Health</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE ADMINISTRATION = yes, LIKE GROUP WORK = yes</t>
+    <t xml:space="preserve">LIKE MANAGEMENT = yes, LIKE GROUP WORK = yes</t>
   </si>
   <si>
     <t xml:space="preserve">Nurse</t>
@@ -402,9 +402,6 @@
     <t xml:space="preserve">Property Management</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE MANAGEMENT = yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">OUTDOOR WORK = no</t>
   </si>
   <si>
@@ -585,7 +582,7 @@
     <t xml:space="preserve">LIKE PHYSICS</t>
   </si>
   <si>
-    <t xml:space="preserve">IF PROFESSION = engineering AND LIKE MATH = yes LIKE MATH = yes, LIKE PHYSICS = yes LIKE PHYSICS = yes THEN AREA = electrical engineering</t>
+    <t xml:space="preserve">IF PROFESSION = engineering LIKE MATH = yes, LIKE PHYSICS = yes THEN AREA = electrical engineering</t>
   </si>
   <si>
     <t xml:space="preserve">LIKE MATH</t>
@@ -639,6 +636,9 @@
     <t xml:space="preserve">IF PROFESSION = science AND LIKE BIOLOGY = yes AND LIKE PHYSICS = yes THEN area = oceanography</t>
   </si>
   <si>
+    <t xml:space="preserve">LIKE LAW</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIKE WRITING</t>
   </si>
   <si>
@@ -696,6 +696,9 @@
     <t xml:space="preserve">IF PROFESSION = medical AND LIKE BIOLOGY = yes AND LIKE CHEMISTRY= yes THEN AREA = general practitioner</t>
   </si>
   <si>
+    <t xml:space="preserve">************************************</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIKE SOIL</t>
   </si>
   <si>
@@ -756,13 +759,13 @@
     <t xml:space="preserve">IF PROFESSION = psychology AND LIKE SOCIAL SCIENCE = yes THEN AREA = mental therapy</t>
   </si>
   <si>
-    <t xml:space="preserve">IF PROFESSION = psychology AND LIKE GROUP WORK = yes AND LIKE ANALYTICAL SKILLS = yes THEN AREA = psychological research</t>
+    <t xml:space="preserve">IF PROFESSION = psychology AND GROUP WORK = yes AND LIKE ANALYTICAL SKILLS = yes THEN AREA = psychological research</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = psychology AND LIKE INTERNSHIPS = yes THEN AREA = industrial psychology</t>
   </si>
   <si>
-    <t xml:space="preserve">IF PROFESSION = psychology AND LIKE GROUP WORK = yes AND LIKE SOCIAL SCIENCE = yes THEN AREA = accessibility</t>
+    <t xml:space="preserve">IF PROFESSION = psychology AND GROUP WORK = yes AND LIKE SOCIAL SCIENCE = yes THEN AREA = accessibility</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = psychology AND LIKE COMMUNICATION = yes, LIKE ANALYTICAL SKILLS = yes THEN AREA = clinical psychology</t>
@@ -786,13 +789,13 @@
     <t xml:space="preserve">IF PROFESSION = health care AND LIKE COMMUNICATION = yes THEN AREA = health services management</t>
   </si>
   <si>
-    <t xml:space="preserve">IF PROFESSION = health care AND LIKE ADMINISTRATION = yes THEN AREA = health care administration</t>
+    <t xml:space="preserve">IF PROFESSION = health care AND LIKE MANAGEMENT = yes THEN AREA = health care administration</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = health care AND LIKE BIOLOGY = yes THEN AREA = physicians assistant</t>
   </si>
   <si>
-    <t xml:space="preserve">IF PROFESSION = health care AND LIKE ADMINISTRATION = yes AND LIKE GROUP WORK = yes THEN AREA = public health</t>
+    <t xml:space="preserve">IF PROFESSION = health care AND LIKE MANAGEMENT = yes AND GROUP WORK = yes THEN AREA = public health</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = health care AND LIKE ANATOMY = yes AND LIKE CHEMISTRY = yes THEN AREA = nursing</t>
@@ -841,6 +844,9 @@
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = cs AND LIKE ORIGINALITY = yes THEN AREA = languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE COMMUNICATION</t>
   </si>
 </sst>
 </file>
@@ -968,7 +974,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1010,6 +1016,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1092,17 +1102,17 @@
   </sheetPr>
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="109.071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="107.724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,16 +1961,16 @@
         <v>125</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="B53" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>39</v>
@@ -1970,27 +1980,27 @@
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>102</v>
@@ -2021,16 +2031,16 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2039,10 +2049,10 @@
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,7 +2061,7 @@
         <v>39</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>39</v>
@@ -2061,20 +2071,20 @@
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -2124,21 +2134,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="109.341836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="107.994897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2166,191 +2176,191 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,32 +2368,32 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2391,12 +2401,12 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,7 +2414,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,12 +2422,12 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,12 +2435,12 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2438,12 +2448,12 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,12 +2461,12 @@
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2464,17 +2474,17 @@
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,7 +2492,7 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,12 +2500,12 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2503,12 +2513,12 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,17 +2526,17 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,29 +2558,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z61"/>
+  <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B61" activeCellId="0" sqref="B61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C241" activeCellId="0" sqref="C241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="131.020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="129.591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>146</v>
-      </c>
       <c r="C1" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2598,81 +2608,105 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>187</v>
+      <c r="C2" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>189</v>
+      <c r="C3" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>191</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>194</v>
+      <c r="C6" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>196</v>
+      <c r="C7" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>198</v>
+      <c r="C8" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>202</v>
+      <c r="C10" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2683,6 +2717,9 @@
       <c r="B12" s="0" t="s">
         <v>206</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -2699,6 +2736,9 @@
       <c r="B14" s="0" t="s">
         <v>210</v>
       </c>
+      <c r="C14" s="0" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -2707,6 +2747,9 @@
       <c r="B15" s="0" t="s">
         <v>212</v>
       </c>
+      <c r="C15" s="0" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -2715,6 +2758,9 @@
       <c r="B16" s="0" t="s">
         <v>214</v>
       </c>
+      <c r="C16" s="0" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -2731,6 +2777,9 @@
       <c r="B18" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="C18" s="0" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -2739,6 +2788,9 @@
       <c r="B19" s="0" t="s">
         <v>219</v>
       </c>
+      <c r="C19" s="0" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -2747,6 +2799,9 @@
       <c r="B20" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="C20" s="0" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -2755,237 +2810,966 @@
       <c r="B21" s="0" t="s">
         <v>223</v>
       </c>
+      <c r="C21" s="0" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>231</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>272</v>
-      </c>
-    </row>
+        <v>273</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C63" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C75" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C98" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C99" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C100" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C101" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C102" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C103" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C104" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C106" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C107" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C108" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C110" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C111" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C114" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C115" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C116" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C118" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C119" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C121" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C123" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C127" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C130" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C135" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C136" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C139" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C140" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C141" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C142" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C143" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C144" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C146" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C147" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C148" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C150" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C151" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C152" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C154" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C155" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C158" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C159" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C161" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C162" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C163" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C166" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C167" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C170" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C171" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C174" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C175" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C176" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C178" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C179" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C180" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C181" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C182" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C183" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C186" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C187" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C188" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C190" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C191" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C192" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C194" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C195" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C196" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C198" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C199" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C200" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C201" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C202" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C203" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C206" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C207" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C210" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C211" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C214" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C215" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C218" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C219" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C221" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C222" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C223" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C224" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C226" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C227" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C228" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C230" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C231" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C234" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C235" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C236" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C238" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C239" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C241" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
stardted updating fc constructor
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1108,11 +1108,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="107.724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="106.510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2134,10 +2134,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="107.994897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="106.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2566,10 +2566,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="129.591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="128.107142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added left hands of rules to fc
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -591,7 +591,7 @@
     <t xml:space="preserve">IF PROFESSION = engineering AND LIKE PHYSICS = yes AND GROUP WORK = yes then AREA = mechanical engineering</t>
   </si>
   <si>
-    <t xml:space="preserve">IF PROFESSION = engineering AND LIKE LAW = yes AND LIKE PHYSICS = yes the AREA = CIVIL</t>
+    <t xml:space="preserve">IF PROFESSION = engineering AND LIKE LAW = yes AND LIKE PHYSICS = yes the AREA = civil</t>
   </si>
   <si>
     <t xml:space="preserve">LIKE BIOLOGY</t>
@@ -669,28 +669,31 @@
     <t xml:space="preserve">IF PROFESSION = business AND GOOD CREDIT = yes, LIKE MANAGEMENT = yes THEN AREA = ceo</t>
   </si>
   <si>
+    <t xml:space="preserve">LIKE READING</t>
+  </si>
+  <si>
     <t xml:space="preserve">IF PROFESSION = medical AND GROUP WORK = yes THEN AREA = mental health</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE READING</t>
+    <t xml:space="preserve">LIKE CLIMATE</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = medical LIKE CHEMISTRY =yes THEN AREA = oncology</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE CLIMATE</t>
+    <t xml:space="preserve">LIKE STONES</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = medical AND STATE LICENSURE = yes AND LIKE chemistry = yes THEN AREA = cardiology</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE STONES</t>
+    <t xml:space="preserve">LIKE LAND</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = medical AND LIKE MEDICAL ETHICS = yes THEN AREA = orthopedics</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE LAND</t>
+    <t xml:space="preserve">LIKE SOIL</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = medical AND LIKE BIOLOGY = yes AND LIKE CHEMISTRY= yes THEN AREA = general practitioner</t>
@@ -699,58 +702,55 @@
     <t xml:space="preserve">************************************</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE SOIL</t>
+    <t xml:space="preserve">LIKE WATER RESOURCES</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = english AND LIKE WRITING = yes AND LIKE ORIGINALITY = yes THEN AREA = author</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE WATER RESOURCES</t>
+    <t xml:space="preserve">LIKE ANALYTICAL SKILLS</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = english AND LIKE MEDIA = yes AND LIKE SOCIAL SCIENCE = yes THEN AREA = journalism</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE ANALYTICAL SKILLS</t>
+    <t xml:space="preserve">LIKE INTERNSHIPS</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = english AND LIKE ENGLISH = yes AND LIKE READING = yes THEN AREA = editing </t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE INTERNSHIPS</t>
+    <t xml:space="preserve">LIKE ANATOMY</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = english AND LIKE MARKETING = yes AND LIKE ENGLISH = yes THEN AREA = copy writing</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE ANATOMY</t>
+    <t xml:space="preserve">LIKE CHILDREN</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = english AND LIKE READING = yes THEN LIKE ORIGINALITY = yes THEN AREA = academia</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE CHILDREN</t>
+    <t xml:space="preserve">RELIABLE</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = geography AND LIKE CLIMATE = yes AND LIKE STONES = yes THEN AREA = precious metals</t>
   </si>
   <si>
-    <t xml:space="preserve">RELIABLE</t>
+    <t xml:space="preserve">LIKE REPAIRS</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = geography AND LIKE LAND = yes AND LIKE ORIGINALITY = yes THEN AREA = cartography</t>
   </si>
   <si>
-    <t xml:space="preserve">LIKE REPAIRS</t>
-  </si>
-  <si>
     <t xml:space="preserve">IF PROFESSION = geography AND LIKE SOIL = yes AND LIKE CLIMATE = yes THEN AREA = climatology</t>
   </si>
   <si>
+    <t xml:space="preserve">AREA</t>
+  </si>
+  <si>
     <t xml:space="preserve">IF PROFESSION = geography AND LIKE WATER RESOURCES = yes AND LIKE SOIL = yes THEN AREA = environmental management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AREA</t>
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = geography AND LIKE MATH = yes THEN AREA = geomatics</t>
@@ -1103,16 +1103,16 @@
   <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="topLeft" activeCell="D45" activeCellId="1" sqref="7:7 D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="106.510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="105.428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,15 +2129,15 @@
   <dimension ref="A1:Z81"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="7:7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="106.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="105.561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,16 +2560,15 @@
   </sheetPr>
   <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C241" activeCellId="0" sqref="C241"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="128.107142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="126.755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,6 +2615,9 @@
       <c r="C2" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -2627,6 +2629,9 @@
       <c r="C3" s="0" t="s">
         <v>187</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -2638,6 +2643,9 @@
       <c r="C4" s="0" t="s">
         <v>185</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -2657,6 +2665,9 @@
       <c r="C6" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2668,6 +2679,9 @@
       <c r="C7" s="0" t="s">
         <v>185</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -2679,6 +2693,9 @@
       <c r="C8" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -2698,6 +2715,9 @@
       <c r="C10" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -2709,6 +2729,9 @@
       <c r="C11" s="0" t="s">
         <v>204</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -2720,6 +2743,9 @@
       <c r="C12" s="0" t="s">
         <v>185</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -2739,6 +2765,9 @@
       <c r="C14" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -2750,6 +2779,9 @@
       <c r="C15" s="0" t="s">
         <v>187</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -2761,137 +2793,167 @@
       <c r="C16" s="0" t="s">
         <v>190</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>192</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>190</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>192</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>190</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>239</v>
+        <v>170</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>240</v>
@@ -2899,24 +2961,30 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>243</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>187</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,138 +2992,174 @@
         <v>244</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>246</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
         <v>247</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D35" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>250</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="0" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
         <v>251</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>252</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="0" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
         <v>253</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>254</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="0" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>255</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D43" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>258</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D46" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
         <v>259</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D47" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>260</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D48" s="0" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>262</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D50" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
         <v>263</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>187</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3075,6 +3179,9 @@
       <c r="C54" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D54" s="0" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
@@ -3083,690 +3190,1032 @@
       <c r="C55" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D55" s="0" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>270</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D58" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
         <v>271</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D59" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
         <v>272</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D60" s="0" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
         <v>273</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D62" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D66" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D67" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D70" s="0" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D71" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D72" s="0" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D74" s="0" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D75" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D78" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D79" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
         <v>192</v>
       </c>
+      <c r="D80" s="0" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="0" t="s">
         <v>205</v>
       </c>
+      <c r="D83" s="0" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="0" t="s">
         <v>207</v>
       </c>
+      <c r="D84" s="0" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
         <v>209</v>
       </c>
+      <c r="D87" s="0" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="0" t="s">
         <v>211</v>
       </c>
+      <c r="D88" s="0" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>89</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="0" t="s">
         <v>213</v>
       </c>
+      <c r="D91" s="0" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>91</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="0" t="s">
         <v>194</v>
       </c>
+      <c r="D95" s="0" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
         <v>213</v>
       </c>
+      <c r="D96" s="0" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D98" s="0" t="n">
+        <v>97</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>98</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="s">
         <v>207</v>
       </c>
+      <c r="D100" s="0" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D102" s="0" t="n">
+        <v>101</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="0" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>103</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D106" s="0" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="0" t="s">
         <v>207</v>
       </c>
+      <c r="D108" s="0" t="n">
+        <v>107</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D110" s="0" t="n">
+        <v>109</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="0" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D114" s="0" t="n">
+        <v>113</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="0" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="0" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>115</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>117</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="0" t="s">
         <v>187</v>
       </c>
+      <c r="D119" s="0" t="n">
+        <v>118</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>121</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="0" t="s">
         <v>211</v>
       </c>
+      <c r="D123" s="0" t="n">
+        <v>122</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D126" s="0" t="n">
+        <v>125</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D127" s="0" t="n">
+        <v>126</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="0" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="D128" s="0" t="n">
+        <v>127</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D130" s="0" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="0" t="s">
-        <v>231</v>
+        <v>230</v>
+      </c>
+      <c r="D131" s="0" t="n">
+        <v>130</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D134" s="0" t="n">
+        <v>133</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D135" s="0" t="n">
+        <v>134</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="0" t="s">
         <v>211</v>
       </c>
+      <c r="D136" s="0" t="n">
+        <v>135</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D138" s="0" t="n">
+        <v>137</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="0" t="s">
         <v>274</v>
       </c>
+      <c r="D139" s="0" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="0" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <v>139</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D142" s="0" t="n">
+        <v>141</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="0" t="s">
         <v>198</v>
       </c>
+      <c r="D143" s="0" t="n">
+        <v>142</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="D144" s="0" t="n">
+        <v>143</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D147" s="0" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="D148" s="0" t="n">
+        <v>147</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D150" s="0" t="n">
+        <v>149</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="D151" s="0" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="0" t="s">
         <v>194</v>
       </c>
+      <c r="D152" s="0" t="n">
+        <v>151</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D154" s="0" t="n">
+        <v>153</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="0" t="s">
         <v>192</v>
       </c>
+      <c r="D155" s="0" t="n">
+        <v>154</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D158" s="0" t="n">
+        <v>157</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="0" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="D159" s="0" t="n">
+        <v>158</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D162" s="0" t="n">
+        <v>161</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="0" t="s">
         <v>274</v>
       </c>
+      <c r="D163" s="0" t="n">
+        <v>162</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D166" s="0" t="n">
+        <v>165</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="D167" s="0" t="n">
+        <v>166</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>169</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="0" t="s">
         <v>190</v>
       </c>
+      <c r="D171" s="0" t="n">
+        <v>170</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>173</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C175" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="D175" s="0" t="n">
+        <v>174</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D176" s="0" t="n">
+        <v>175</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C178" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D178" s="0" t="n">
+        <v>177</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C179" s="0" t="s">
-        <v>233</v>
+        <v>232</v>
+      </c>
+      <c r="D179" s="0" t="n">
+        <v>178</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C180" s="0" t="s">
         <v>192</v>
       </c>
+      <c r="D180" s="0" t="n">
+        <v>179</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C182" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D182" s="0" t="n">
+        <v>181</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C183" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="D183" s="0" t="n">
+        <v>182</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C186" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="D186" s="0" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C187" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="D187" s="0" t="n">
+        <v>186</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C188" s="0" t="s">
         <v>274</v>
       </c>
+      <c r="D188" s="0" t="n">
+        <v>187</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D190" s="0" t="n">
+        <v>189</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C191" s="0" t="s">
         <v>187</v>
       </c>
+      <c r="D191" s="0" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C192" s="0" t="s">
         <v>192</v>
       </c>
+      <c r="D192" s="0" t="n">
+        <v>191</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C194" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D194" s="0" t="n">
+        <v>193</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C195" s="0" t="s">
         <v>274</v>
       </c>
+      <c r="D195" s="0" t="n">
+        <v>194</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C196" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="D196" s="0" t="n">
+        <v>195</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C198" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D198" s="0" t="n">
+        <v>197</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C199" s="0" t="s">
         <v>211</v>
       </c>
+      <c r="D199" s="0" t="n">
+        <v>198</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C200" s="0" t="s">
         <v>274</v>
       </c>
+      <c r="D200" s="0" t="n">
+        <v>199</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C201" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C202" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D202" s="0" t="n">
+        <v>201</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C203" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="D203" s="0" t="n">
+        <v>202</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C206" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="D206" s="0" t="n">
+        <v>205</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D207" s="0" t="n">
+        <v>206</v>
+      </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C210" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D210" s="0" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C211" s="0" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>236</v>
+      </c>
+      <c r="D211" s="0" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C214" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D214" s="0" t="n">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C215" s="0" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>238</v>
+      </c>
+      <c r="D215" s="0" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C218" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D218" s="0" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C219" s="0" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D219" s="0" t="n">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C221" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C222" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D222" s="0" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C223" s="0" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D223" s="0" t="n">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C224" s="0" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D224" s="0" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C226" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D226" s="0" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C227" s="0" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D227" s="0" t="n">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C228" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="D228" s="0" t="n">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C230" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D230" s="0" t="n">
         <v>229</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C230" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C231" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D231" s="0" t="n">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C234" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D234" s="0" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C235" s="0" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D235" s="0" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C236" s="0" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D236" s="0" t="n">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C238" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D238" s="0" t="n">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C239" s="0" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D239" s="0" t="n">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C241" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
converted ifconditions method of fc to use private comparison function
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="275">
   <si>
     <t xml:space="preserve">Profession</t>
   </si>
@@ -756,6 +757,9 @@
     <t xml:space="preserve">IF PROFESSION = geography AND LIKE MATH = yes THEN AREA = geomatics</t>
   </si>
   <si>
+    <t xml:space="preserve">LIKE COMMUNICATION</t>
+  </si>
+  <si>
     <t xml:space="preserve">IF PROFESSION = psychology AND LIKE SOCIAL SCIENCE = yes THEN AREA = mental therapy</t>
   </si>
   <si>
@@ -844,9 +848,6 @@
   </si>
   <si>
     <t xml:space="preserve">IF PROFESSION = cs AND LIKE ORIGINALITY = yes THEN AREA = languages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIKE COMMUNICATION</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1104,7 @@
   <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="1" sqref="7:7 D45"/>
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2129,7 +2130,7 @@
   <dimension ref="A1:Z81"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="7:7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2560,8 +2561,8 @@
   </sheetPr>
   <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2988,18 +2989,21 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>244</v>
+      </c>
       <c r="B32" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>170</v>
@@ -3010,7 +3014,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>185</v>
@@ -3021,17 +3025,17 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>170</v>
@@ -3042,7 +3046,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>190</v>
@@ -3053,7 +3057,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>185</v>
@@ -3064,7 +3068,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>225</v>
@@ -3072,7 +3076,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>170</v>
@@ -3083,7 +3087,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>198</v>
@@ -3094,17 +3098,17 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>170</v>
@@ -3115,7 +3119,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>194</v>
@@ -3126,7 +3130,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>196</v>
@@ -3137,12 +3141,12 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>170</v>
@@ -3153,7 +3157,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>187</v>
@@ -3164,17 +3168,17 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>170</v>
@@ -3185,7 +3189,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>158</v>
@@ -3196,17 +3200,17 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>170</v>
@@ -3217,7 +3221,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>198</v>
@@ -3228,7 +3232,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>196</v>
@@ -3239,7 +3243,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>225</v>
@@ -3678,7 +3682,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="0" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="D139" s="0" t="n">
         <v>138</v>
@@ -3816,7 +3820,7 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="0" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="D163" s="0" t="n">
         <v>162</v>
@@ -3941,7 +3945,7 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C188" s="0" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="D188" s="0" t="n">
         <v>187</v>
@@ -3981,7 +3985,7 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C195" s="0" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="D195" s="0" t="n">
         <v>194</v>
@@ -4013,7 +4017,7 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C200" s="0" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="D200" s="0" t="n">
         <v>199</v>
@@ -4098,7 +4102,7 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C219" s="0" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="D219" s="0" t="n">
         <v>218</v>
@@ -4228,4 +4232,30 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made private methods private
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -1104,7 +1104,7 @@
   <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="topLeft" activeCell="D45" activeCellId="1" sqref="19:19 D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2130,7 +2130,7 @@
   <dimension ref="A1:Z81"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="19:19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2561,8 +2561,8 @@
   </sheetPr>
   <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="19:19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4242,7 +4242,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="19:19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
added pretty printing methods to fc
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -5,13 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1020,7 +1019,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1103,16 +1102,17 @@
   </sheetPr>
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="104.214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="103"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2128,15 +2128,16 @@
   </sheetPr>
   <dimension ref="A1:Z81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="104.34693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="103.132653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,21 +2558,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z241"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="125.270408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="123.923469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="4" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
         <v>144</v>
       </c>
@@ -2606,1622 +2607,1621 @@
       <c r="Z1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="C2" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="4" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="C6" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="4" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="4" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D10" s="0" t="n">
+      <c r="C10" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="4" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="4" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="4" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="C14" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="4" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="4" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="4" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="4" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D18" s="0" t="n">
+      <c r="C18" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="4" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="4" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="4" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="0" t="n">
+      <c r="C22" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="4" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="4" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="4" t="s">
         <v>233</v>
       </c>
       <c r="C25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" s="0" t="n">
+      <c r="C26" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="4" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="4" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="4" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="A29" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="0" t="n">
+      <c r="C30" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="4" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="4" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="4" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D34" s="0" t="n">
+      <c r="C34" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34" s="4" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="4" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="4" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="4" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D38" s="0" t="n">
+      <c r="C38" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38" s="4" t="n">
         <v>37</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="4" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="4" t="n">
         <v>39</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D42" s="0" t="n">
+      <c r="C42" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42" s="4" t="n">
         <v>41</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="4" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="4" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="4" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D46" s="0" t="n">
+      <c r="C46" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="4" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47" s="4" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="4" t="n">
         <v>47</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="4" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C50" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D50" s="0" t="n">
+      <c r="C50" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" s="4" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D51" s="0" t="n">
+      <c r="D51" s="4" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="4" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D54" s="0" t="n">
+      <c r="C54" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" s="4" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55" s="4" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="4" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="4" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D58" s="0" t="n">
+      <c r="C58" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D58" s="4" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D59" s="0" t="n">
+      <c r="D59" s="4" t="n">
         <v>58</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D60" s="0" t="n">
+      <c r="D60" s="4" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D62" s="0" t="n">
+      <c r="C62" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="4" t="n">
         <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D63" s="4" t="n">
         <v>62</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D66" s="0" t="n">
+      <c r="C66" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D66" s="4" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D67" s="4" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D70" s="0" t="n">
+      <c r="C70" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D70" s="4" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D71" s="0" t="n">
+      <c r="D71" s="4" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D72" s="0" t="n">
+      <c r="D72" s="4" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C74" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D74" s="0" t="n">
+      <c r="C74" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D74" s="4" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C75" s="0" t="s">
+      <c r="C75" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D75" s="0" t="n">
+      <c r="D75" s="4" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D78" s="0" t="n">
+      <c r="C78" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D78" s="4" t="n">
         <v>77</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="0" t="s">
+      <c r="C79" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D79" s="0" t="n">
+      <c r="D79" s="4" t="n">
         <v>78</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="0" t="s">
+      <c r="C80" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D80" s="0" t="n">
+      <c r="D80" s="4" t="n">
         <v>79</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C81" s="0" t="s">
+      <c r="C81" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D82" s="0" t="n">
+      <c r="C82" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D82" s="4" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D83" s="0" t="n">
+      <c r="D83" s="4" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D84" s="0" t="n">
+      <c r="D84" s="4" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D86" s="0" t="n">
+      <c r="C86" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D86" s="4" t="n">
         <v>85</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="0" t="s">
+      <c r="C87" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D87" s="0" t="n">
+      <c r="D87" s="4" t="n">
         <v>86</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="0" t="s">
+      <c r="C88" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D88" s="0" t="n">
+      <c r="D88" s="4" t="n">
         <v>87</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D90" s="0" t="n">
+      <c r="C90" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D90" s="4" t="n">
         <v>89</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="0" t="s">
+      <c r="C91" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D91" s="0" t="n">
+      <c r="D91" s="4" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="0" t="s">
+      <c r="C92" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D92" s="0" t="n">
+      <c r="D92" s="4" t="n">
         <v>91</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D94" s="0" t="n">
+      <c r="C94" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D94" s="4" t="n">
         <v>93</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="0" t="s">
+      <c r="C95" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D95" s="0" t="n">
+      <c r="D95" s="4" t="n">
         <v>94</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C96" s="0" t="s">
+      <c r="C96" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D96" s="0" t="n">
+      <c r="D96" s="4" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D98" s="0" t="n">
+      <c r="C98" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D98" s="4" t="n">
         <v>97</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C99" s="0" t="s">
+      <c r="C99" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D99" s="0" t="n">
+      <c r="D99" s="4" t="n">
         <v>98</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C100" s="0" t="s">
+      <c r="C100" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D100" s="0" t="n">
+      <c r="D100" s="4" t="n">
         <v>99</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C101" s="0" t="s">
+      <c r="C101" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D102" s="0" t="n">
+      <c r="C102" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D102" s="4" t="n">
         <v>101</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="0" t="s">
+      <c r="C103" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D103" s="0" t="n">
+      <c r="D103" s="4" t="n">
         <v>102</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C104" s="0" t="s">
+      <c r="C104" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D104" s="0" t="n">
+      <c r="D104" s="4" t="n">
         <v>103</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C106" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D106" s="0" t="n">
+      <c r="C106" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D106" s="4" t="n">
         <v>105</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="0" t="s">
+      <c r="C107" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D107" s="0" t="n">
+      <c r="D107" s="4" t="n">
         <v>106</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C108" s="0" t="s">
+      <c r="C108" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D108" s="0" t="n">
+      <c r="D108" s="4" t="n">
         <v>107</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D110" s="0" t="n">
+      <c r="C110" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D110" s="4" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C111" s="0" t="s">
+      <c r="C111" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D111" s="0" t="n">
+      <c r="D111" s="4" t="n">
         <v>110</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="0" t="s">
+      <c r="C112" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D112" s="0" t="n">
+      <c r="D112" s="4" t="n">
         <v>111</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D114" s="0" t="n">
+      <c r="C114" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D114" s="4" t="n">
         <v>113</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="0" t="s">
+      <c r="C115" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D115" s="0" t="n">
+      <c r="D115" s="4" t="n">
         <v>114</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C116" s="0" t="s">
+      <c r="C116" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D116" s="0" t="n">
+      <c r="D116" s="4" t="n">
         <v>115</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D118" s="0" t="n">
+      <c r="C118" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D118" s="4" t="n">
         <v>117</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="0" t="s">
+      <c r="C119" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D119" s="0" t="n">
+      <c r="D119" s="4" t="n">
         <v>118</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="0" t="s">
+      <c r="C121" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D122" s="0" t="n">
+      <c r="C122" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D122" s="4" t="n">
         <v>121</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C123" s="0" t="s">
+      <c r="C123" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D123" s="0" t="n">
+      <c r="D123" s="4" t="n">
         <v>122</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D126" s="0" t="n">
+      <c r="C126" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D126" s="4" t="n">
         <v>125</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="0" t="s">
+      <c r="C127" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D127" s="0" t="n">
+      <c r="D127" s="4" t="n">
         <v>126</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="0" t="s">
+      <c r="C128" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D128" s="0" t="n">
+      <c r="D128" s="4" t="n">
         <v>127</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C130" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D130" s="0" t="n">
+      <c r="C130" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D130" s="4" t="n">
         <v>129</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C131" s="0" t="s">
+      <c r="C131" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D131" s="0" t="n">
+      <c r="D131" s="4" t="n">
         <v>130</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D134" s="0" t="n">
+      <c r="C134" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D134" s="4" t="n">
         <v>133</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="0" t="s">
+      <c r="C135" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D135" s="0" t="n">
+      <c r="D135" s="4" t="n">
         <v>134</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C136" s="0" t="s">
+      <c r="C136" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D136" s="0" t="n">
+      <c r="D136" s="4" t="n">
         <v>135</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D138" s="0" t="n">
+      <c r="C138" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D138" s="4" t="n">
         <v>137</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="0" t="s">
+      <c r="C139" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D139" s="0" t="n">
+      <c r="D139" s="4" t="n">
         <v>138</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C140" s="0" t="s">
+      <c r="C140" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D140" s="0" t="n">
+      <c r="D140" s="4" t="n">
         <v>139</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C141" s="0" t="s">
+      <c r="C141" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C142" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D142" s="0" t="n">
+      <c r="C142" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D142" s="4" t="n">
         <v>141</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C143" s="0" t="s">
+      <c r="C143" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D143" s="0" t="n">
+      <c r="D143" s="4" t="n">
         <v>142</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C144" s="0" t="s">
+      <c r="C144" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D144" s="0" t="n">
+      <c r="D144" s="4" t="n">
         <v>143</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C146" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D146" s="0" t="n">
+      <c r="C146" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D146" s="4" t="n">
         <v>145</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="0" t="s">
+      <c r="C147" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D147" s="0" t="n">
+      <c r="D147" s="4" t="n">
         <v>146</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C148" s="0" t="s">
+      <c r="C148" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D148" s="0" t="n">
+      <c r="D148" s="4" t="n">
         <v>147</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C150" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D150" s="0" t="n">
+      <c r="C150" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D150" s="4" t="n">
         <v>149</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="0" t="s">
+      <c r="C151" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D151" s="0" t="n">
+      <c r="D151" s="4" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C152" s="0" t="s">
+      <c r="C152" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D152" s="0" t="n">
+      <c r="D152" s="4" t="n">
         <v>151</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C154" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D154" s="0" t="n">
+      <c r="C154" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D154" s="4" t="n">
         <v>153</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C155" s="0" t="s">
+      <c r="C155" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D155" s="0" t="n">
+      <c r="D155" s="4" t="n">
         <v>154</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C158" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D158" s="0" t="n">
+      <c r="C158" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D158" s="4" t="n">
         <v>157</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C159" s="0" t="s">
+      <c r="C159" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D159" s="0" t="n">
+      <c r="D159" s="4" t="n">
         <v>158</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="0" t="s">
+      <c r="C161" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D162" s="0" t="n">
+      <c r="C162" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D162" s="4" t="n">
         <v>161</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="0" t="s">
+      <c r="C163" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D163" s="0" t="n">
+      <c r="D163" s="4" t="n">
         <v>162</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C166" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D166" s="0" t="n">
+      <c r="C166" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D166" s="4" t="n">
         <v>165</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C167" s="0" t="s">
+      <c r="C167" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D167" s="0" t="n">
+      <c r="D167" s="4" t="n">
         <v>166</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C170" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D170" s="0" t="n">
+      <c r="C170" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D170" s="4" t="n">
         <v>169</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="0" t="s">
+      <c r="C171" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D171" s="0" t="n">
+      <c r="D171" s="4" t="n">
         <v>170</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C174" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D174" s="0" t="n">
+      <c r="C174" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D174" s="4" t="n">
         <v>173</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C175" s="0" t="s">
+      <c r="C175" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D175" s="0" t="n">
+      <c r="D175" s="4" t="n">
         <v>174</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C176" s="0" t="s">
+      <c r="C176" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D176" s="0" t="n">
+      <c r="D176" s="4" t="n">
         <v>175</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D178" s="0" t="n">
+      <c r="C178" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D178" s="4" t="n">
         <v>177</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C179" s="0" t="s">
+      <c r="C179" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D179" s="0" t="n">
+      <c r="D179" s="4" t="n">
         <v>178</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C180" s="0" t="s">
+      <c r="C180" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D180" s="0" t="n">
+      <c r="D180" s="4" t="n">
         <v>179</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C181" s="0" t="s">
+      <c r="C181" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C182" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D182" s="0" t="n">
+      <c r="C182" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D182" s="4" t="n">
         <v>181</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="0" t="s">
+      <c r="C183" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D183" s="0" t="n">
+      <c r="D183" s="4" t="n">
         <v>182</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D186" s="0" t="n">
+      <c r="C186" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D186" s="4" t="n">
         <v>185</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C187" s="0" t="s">
+      <c r="C187" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D187" s="0" t="n">
+      <c r="D187" s="4" t="n">
         <v>186</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C188" s="0" t="s">
+      <c r="C188" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D188" s="0" t="n">
+      <c r="D188" s="4" t="n">
         <v>187</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C190" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D190" s="0" t="n">
+      <c r="C190" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D190" s="4" t="n">
         <v>189</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C191" s="0" t="s">
+      <c r="C191" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D191" s="0" t="n">
+      <c r="D191" s="4" t="n">
         <v>190</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="0" t="s">
+      <c r="C192" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D192" s="0" t="n">
+      <c r="D192" s="4" t="n">
         <v>191</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C194" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D194" s="0" t="n">
+      <c r="C194" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D194" s="4" t="n">
         <v>193</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="0" t="s">
+      <c r="C195" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D195" s="0" t="n">
+      <c r="D195" s="4" t="n">
         <v>194</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C196" s="0" t="s">
+      <c r="C196" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D196" s="0" t="n">
+      <c r="D196" s="4" t="n">
         <v>195</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C198" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D198" s="0" t="n">
+      <c r="C198" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D198" s="4" t="n">
         <v>197</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C199" s="0" t="s">
+      <c r="C199" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D199" s="0" t="n">
+      <c r="D199" s="4" t="n">
         <v>198</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C200" s="0" t="s">
+      <c r="C200" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D200" s="0" t="n">
+      <c r="D200" s="4" t="n">
         <v>199</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C201" s="0" t="s">
+      <c r="C201" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C202" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D202" s="0" t="n">
+      <c r="C202" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D202" s="4" t="n">
         <v>201</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C203" s="0" t="s">
+      <c r="C203" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D203" s="0" t="n">
+      <c r="D203" s="4" t="n">
         <v>202</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D206" s="0" t="n">
+      <c r="C206" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D206" s="4" t="n">
         <v>205</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="0" t="s">
+      <c r="C207" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D207" s="0" t="n">
+      <c r="D207" s="4" t="n">
         <v>206</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C210" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D210" s="0" t="n">
+      <c r="C210" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D210" s="4" t="n">
         <v>209</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C211" s="0" t="s">
+      <c r="C211" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="D211" s="0" t="n">
+      <c r="D211" s="4" t="n">
         <v>210</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D214" s="0" t="n">
+      <c r="C214" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D214" s="4" t="n">
         <v>213</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="0" t="s">
+      <c r="C215" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D215" s="0" t="n">
+      <c r="D215" s="4" t="n">
         <v>214</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D218" s="0" t="n">
+      <c r="C218" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D218" s="4" t="n">
         <v>217</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="0" t="s">
+      <c r="C219" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D219" s="0" t="n">
+      <c r="D219" s="4" t="n">
         <v>218</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C221" s="0" t="s">
+      <c r="C221" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D222" s="0" t="n">
+      <c r="C222" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D222" s="4" t="n">
         <v>221</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C223" s="0" t="s">
+      <c r="C223" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D223" s="0" t="n">
+      <c r="D223" s="4" t="n">
         <v>222</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="0" t="s">
+      <c r="C224" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D224" s="0" t="n">
+      <c r="D224" s="4" t="n">
         <v>223</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C226" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D226" s="0" t="n">
+      <c r="C226" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D226" s="4" t="n">
         <v>225</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="0" t="s">
+      <c r="C227" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D227" s="0" t="n">
+      <c r="D227" s="4" t="n">
         <v>226</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C228" s="0" t="s">
+      <c r="C228" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D228" s="0" t="n">
+      <c r="D228" s="4" t="n">
         <v>227</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C230" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D230" s="0" t="n">
+      <c r="C230" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D230" s="4" t="n">
         <v>229</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C231" s="0" t="s">
+      <c r="C231" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D231" s="0" t="n">
+      <c r="D231" s="4" t="n">
         <v>230</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C234" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D234" s="0" t="n">
+      <c r="C234" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D234" s="4" t="n">
         <v>233</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="0" t="s">
+      <c r="C235" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D235" s="0" t="n">
+      <c r="D235" s="4" t="n">
         <v>234</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C236" s="0" t="s">
+      <c r="C236" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D236" s="0" t="n">
+      <c r="D236" s="4" t="n">
         <v>235</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C238" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D238" s="0" t="n">
+      <c r="C238" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D238" s="4" t="n">
         <v>237</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C239" s="0" t="s">
+      <c r="C239" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D239" s="0" t="n">
+      <c r="D239" s="4" t="n">
         <v>238</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C241" s="0" t="s">
+      <c r="C241" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4231,30 +4231,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected major array boundary in bc
</commit_message>
<xml_diff>
--- a/project1_knowledge.xlsx
+++ b/project1_knowledge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -862,7 +862,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -883,21 +882,18 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1103,7 +1099,7 @@
   <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="topLeft" activeCell="D45" activeCellId="1" sqref="B22:B26 D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2128,14 +2124,14 @@
   </sheetPr>
   <dimension ref="A1:Z81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="B22:B26 A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="103.132653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="136.852040816327"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
@@ -2560,8 +2556,8 @@
   </sheetPr>
   <dimension ref="A1:Z241"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>